<commit_message>
Update used prices for Mn, Ni and Li
</commit_message>
<xml_diff>
--- a/example notebooks/Example publication - integrated modelling/data/ODYM_database/3_PR_mineral_price_v1.xlsx
+++ b/example notebooks/Example publication - integrated modelling/data/ODYM_database/3_PR_mineral_price_v1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="455" documentId="13_ncr:1_{211C751D-FD5C-4197-97D0-0E32C9E58A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB56F910-378A-4292-9F4F-6CB8AE7D17E9}"/>
+  <xr:revisionPtr revIDLastSave="475" documentId="13_ncr:1_{211C751D-FD5C-4197-97D0-0E32C9E58A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAE5DB56-7342-4AD8-A6AA-BF1AC0076211}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -303,12 +303,6 @@
     <t>SMM (CoSO)</t>
   </si>
   <si>
-    <t>SMM (LiCO)</t>
-  </si>
-  <si>
-    <t>Source current (4-1-2022)</t>
-  </si>
-  <si>
     <t>LME, 3 month contract</t>
   </si>
   <si>
@@ -365,6 +359,12 @@
   <si>
     <t>used</t>
   </si>
+  <si>
+    <t>Source current (13/05/2022)</t>
+  </si>
+  <si>
+    <t>SMM (LiCO battery grade)</t>
+  </si>
 </sst>
 </file>
 
@@ -376,7 +376,7 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +485,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF303133"/>
+      <name val="Lato"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -607,7 +613,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -637,6 +643,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1382,10 +1389,10 @@
         <v>59</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>41</v>
@@ -1552,7 +1559,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,7 +1583,7 @@
         <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
         <v>80</v>
@@ -1585,7 +1592,7 @@
         <v>81</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1596,7 +1603,7 @@
         <v>7.0529902282149903</v>
       </c>
       <c r="C2" s="20">
-        <v>24.393108745506282</v>
+        <v>30.339662318095858</v>
       </c>
       <c r="D2">
         <v>65.131491595786798</v>
@@ -1631,7 +1638,7 @@
         <v>84</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1651,10 +1658,10 @@
         <v>75</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1677,7 +1684,7 @@
         <v>83</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -1702,7 +1709,7 @@
         <v>76</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -1724,10 +1731,10 @@
         <v>75</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -1740,10 +1747,10 @@
         <v>22.484375592672301</v>
       </c>
       <c r="C8" s="20">
-        <v>225.48015209623978</v>
+        <v>361.78168514046973</v>
       </c>
       <c r="D8" s="20">
-        <v>225.48015209623978</v>
+        <v>361.78168514046973</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>75</v>
@@ -1752,7 +1759,7 @@
         <v>82</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
@@ -1764,7 +1771,7 @@
       <c r="B9">
         <v>1.1683256580000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="20">
         <v>3.2220599999999999</v>
       </c>
       <c r="D9">
@@ -1774,10 +1781,10 @@
         <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
@@ -1790,7 +1797,7 @@
         <v>3.3093300170059199</v>
       </c>
       <c r="C10" s="20">
-        <v>4.8224832027012265</v>
+        <v>3.6701079942116572</v>
       </c>
       <c r="D10">
         <v>14.605292342160901</v>
@@ -1799,7 +1806,7 @@
         <v>75</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>86</v>
@@ -1814,7 +1821,7 @@
         <v>8.9002478097115993</v>
       </c>
       <c r="C11" s="21">
-        <v>76.316522152274615</v>
+        <v>72.356696306924817</v>
       </c>
       <c r="D11">
         <v>114.22530937582999</v>
@@ -1823,7 +1830,7 @@
         <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>87</v>
@@ -1843,18 +1850,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A2C87C-7A4D-47BE-AC2C-75D177C255A0}">
   <dimension ref="A1:W265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="E267" sqref="E267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>67</v>
@@ -11982,7 +11989,7 @@
   <dimension ref="A1:AQ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12060,7 +12067,7 @@
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="19">
         <v>0.66534994212199805</v>
@@ -12151,7 +12158,7 @@
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R4" s="19"/>
       <c r="S4" s="19"/>
@@ -12168,8 +12175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC49B553-C171-4139-98F0-0A2F66A37369}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12207,7 +12214,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19">
@@ -12220,7 +12227,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -12283,8 +12290,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="23">
+        <v>10</v>
+      </c>
+      <c r="C11" s="20">
+        <f>B11/B2</f>
+        <v>53.226984584353843</v>
+      </c>
       <c r="D11" s="20"/>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>

</xml_diff>